<commit_message>
Updated TodoList & Added SceneManager
</commit_message>
<xml_diff>
--- a/TodoList.xlsx
+++ b/TodoList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\Unity\VR-Journalism-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Unity\VR-Journalism-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AD28A7-3E88-4E5B-9B90-C5F4EC7AD2A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37775332-39EB-4B86-8865-E7C6A4FD889D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{A0D18156-EC0B-421E-B77C-FCCB5F8E7D12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0D18156-EC0B-421E-B77C-FCCB5F8E7D12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>VR Journalism Project</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>VR Controls</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Friday 15</t>
+  </si>
+  <si>
+    <t>Thursday 14</t>
   </si>
 </sst>
 </file>
@@ -195,7 +204,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +236,11 @@
         <fgColor theme="8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -255,7 +269,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -264,8 +278,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -297,19 +312,23 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="5" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
     <cellStyle name="Accent3" xfId="5" builtinId="37"/>
     <cellStyle name="Accent4" xfId="6" builtinId="41"/>
     <cellStyle name="Accent5" xfId="7" builtinId="45"/>
+    <cellStyle name="Accent6" xfId="8" builtinId="49"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -566,24 +585,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261EE6D3-1E41-43EF-8299-B62A2DD2C0DD}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.375" customWidth="1"/>
-    <col min="2" max="2" width="17.375" customWidth="1"/>
+    <col min="1" max="1" width="2.3984375" customWidth="1"/>
+    <col min="2" max="2" width="17.3984375" customWidth="1"/>
     <col min="3" max="3" width="52" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="12.3984375" customWidth="1"/>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.875" customWidth="1"/>
-    <col min="7" max="9" width="11" customWidth="1"/>
+    <col min="6" max="6" width="2.8984375" customWidth="1"/>
+    <col min="7" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45.75" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:10" ht="45.6" x14ac:dyDescent="0.8">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -593,7 +612,7 @@
       <c r="E1" s="15"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -611,7 +630,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="33.75" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="28.2" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -625,21 +644,24 @@
       <c r="E3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -652,22 +674,26 @@
       <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="17"/>
-    </row>
-    <row r="6" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -680,21 +706,25 @@
       <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="17"/>
-    </row>
-    <row r="7" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="F6" s="16"/>
+    </row>
+    <row r="7" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="17"/>
-    </row>
-    <row r="8" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
         <v>12</v>
@@ -705,23 +735,29 @@
       <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="E8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="17"/>
-    </row>
-    <row r="10" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="D9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
       <c r="B10" s="2" t="s">
         <v>42</v>
       </c>
@@ -730,17 +766,17 @@
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="17"/>
-    </row>
-    <row r="12" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -748,7 +784,7 @@
       <c r="E12" s="14"/>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
         <v>14</v>
@@ -762,104 +798,104 @@
       <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="F16" s="19"/>
+    </row>
+    <row r="17" spans="2:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C18" s="11"/>
-      <c r="F18" s="16"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="19"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C19" s="11"/>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C20" s="11"/>
-      <c r="F20" s="16"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F20" s="19"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C21" s="11"/>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C22" s="11"/>
-      <c r="F22" s="16"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F22" s="19"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C23" s="11"/>
-      <c r="F23" s="16"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C24" s="11"/>
-      <c r="F24" s="16"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F24" s="19"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C25" s="11"/>
-      <c r="F25" s="16"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F25" s="19"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C26" s="11"/>
-      <c r="F26" s="16"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F26" s="19"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27" s="11"/>
-      <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F27" s="19"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C28" s="11"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C29" s="11"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F33" s="6"/>
     </row>
   </sheetData>

</xml_diff>